<commit_message>
prrima prova paolo 1
</commit_message>
<xml_diff>
--- a/Firmware Sistema/Sistema Pylon Rev2 18-07/Tavola Dei Canali Rev2.xlsx
+++ b/Firmware Sistema/Sistema Pylon Rev2 18-07/Tavola Dei Canali Rev2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Giacomo\Elettronica\Github_Repository\Sistema_Pylon\Firmware Sistema\Sistema Pylon Rev2 18-07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBEF755-4D78-43B1-82C7-DBD58CE2D558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888501A9-C173-438D-9A07-8B2C0C80923E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{74CC8E9D-622E-4FE5-A796-FCE34E7CBF94}"/>
   </bookViews>
@@ -541,7 +541,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>